<commit_message>
ander cap berekening VTI-VXUS
</commit_message>
<xml_diff>
--- a/Vanguard US/Vanguard-US-KostenBepaling.xlsx
+++ b/Vanguard US/Vanguard-US-KostenBepaling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7c741cee80ec8cf3/Financieel/IndexFondsenOnderzoek/KeuzeWelkIndexFonds/OnderzoekPerFonds/Vanguard US/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="719" documentId="13_ncr:1_{1145E7EB-B52A-4035-9DB0-6756A4D32375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D8DC6F4-442A-481A-ABFE-5D703243C66C}"/>
+  <xr:revisionPtr revIDLastSave="734" documentId="13_ncr:1_{1145E7EB-B52A-4035-9DB0-6756A4D32375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2706EBA7-5B08-4184-ADC7-E1BEBEAA0344}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -196,7 +196,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="67">
   <si>
     <t>Dividend income</t>
   </si>
@@ -360,9 +360,6 @@
     <t>FTSE USA All Cap</t>
   </si>
   <si>
-    <t>Data as at: 31 March 2021</t>
-  </si>
-  <si>
     <t>Future costs estimation WO dividendleak</t>
   </si>
   <si>
@@ -394,6 +391,12 @@
   </si>
   <si>
     <t>Index data</t>
+  </si>
+  <si>
+    <t>Data as at: 31 Jun 2021</t>
+  </si>
+  <si>
+    <t>CRSP US Total Market Index</t>
   </si>
 </sst>
 </file>
@@ -842,7 +845,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7D6687D-2650-40D8-BB0F-4784280BA24F}">
-  <dimension ref="B2:H20"/>
+  <dimension ref="B2:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -864,10 +867,10 @@
         <v>51</v>
       </c>
       <c r="C2" s="7">
-        <v>69827178</v>
+        <v>75163286</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H2" s="3"/>
     </row>
@@ -876,14 +879,14 @@
         <v>53</v>
       </c>
       <c r="C3" s="7">
-        <v>39813246</v>
+        <v>43376587</v>
       </c>
       <c r="D3" s="6">
         <f>C3/C2</f>
-        <v>0.57016833760631136</v>
+        <v>0.57709806620216153</v>
       </c>
       <c r="F3" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -891,66 +894,68 @@
         <v>52</v>
       </c>
       <c r="C4" s="7">
-        <v>30013932</v>
+        <v>31786699</v>
       </c>
       <c r="D4" s="6">
         <f>C4/C2</f>
-        <v>0.42983166239368858</v>
+        <v>0.42290193379783847</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G5" s="5"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="7">
+        <v>44358982</v>
+      </c>
+      <c r="D6" s="6">
+        <f>C6/C8</f>
+        <v>0.58255414381283166</v>
+      </c>
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="7">
+        <v>31786699</v>
+      </c>
+      <c r="D7" s="6">
+        <f>C7/C8</f>
+        <v>0.4174458561871684</v>
+      </c>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="7">
+        <f>SUM(C6:C7)</f>
+        <v>76145681</v>
+      </c>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C10" s="5">
         <f>VT!C26</f>
         <v>5.2730993928290092E-4</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" s="5">
-        <f>(D3*VTI!C22)+(D4*VXUS!C26)</f>
-        <v>1.6674536306345603E-4</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="6"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" s="4">
-        <f>C7-C8</f>
-        <v>3.6056457621944489E-4</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="6"/>
-    </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" s="33">
-        <f>VT!J12</f>
-        <v>4.6003640353216309E-2</v>
+        <v>55</v>
+      </c>
+      <c r="C11" s="5">
+        <f>(D3*VTI!C22)+(D4*VXUS!C26)</f>
+        <v>1.6594182976464758E-4</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -958,11 +963,11 @@
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" s="33">
-        <f>D4*VXUS!J12</f>
-        <v>3.3092330113641752E-2</v>
+        <v>58</v>
+      </c>
+      <c r="C12" s="4">
+        <f>C10-C11</f>
+        <v>3.6136810951825334E-4</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -977,11 +982,11 @@
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" s="4">
-        <f>VT!J13</f>
-        <v>1.1840408681430441E-3</v>
+        <v>59</v>
+      </c>
+      <c r="C14" s="33">
+        <f>VT!J12</f>
+        <v>4.6003640353216309E-2</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -989,42 +994,73 @@
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C15" s="4">
-        <f>D4*VXUS!J13</f>
-        <v>1.040941452213853E-3</v>
+        <v>60</v>
+      </c>
+      <c r="C15" s="33">
+        <f>D4*VXUS!J12</f>
+        <v>3.2558816912183416E-2</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="6"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="4">
-        <f>C14-C15</f>
-        <v>1.4309941592919109E-4</v>
-      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="4"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="6"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="2"/>
-      <c r="C17" s="4"/>
+      <c r="B17" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="4">
+        <f>VT!J13</f>
+        <v>1.1840408681430441E-3</v>
+      </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="6"/>
     </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="4">
+        <f>D4*VXUS!J13</f>
+        <v>1.0241594364176197E-3</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="6"/>
+    </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="32" t="s">
-        <v>62</v>
-      </c>
+      <c r="B19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="4">
+        <f>C17-C18</f>
+        <v>1.5988143172542446E-4</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="6"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="32"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="6"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="32" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1220,7 +1256,7 @@
       </c>
       <c r="J10" s="5"/>
       <c r="L10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
@@ -1548,7 +1584,7 @@
         <v>9.8333333333333345E-4</v>
       </c>
       <c r="L6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
@@ -1882,7 +1918,7 @@
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C26" s="12">
         <f>C25-AVERAGE(H17:I17)</f>
@@ -2145,7 +2181,7 @@
       </c>
       <c r="J10" s="5"/>
       <c r="L10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
@@ -2407,7 +2443,7 @@
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C26" s="9">
         <f>C25-AVERAGE(H17:I17)</f>

</xml_diff>

<commit_message>
Clean Vanguard US sheet
</commit_message>
<xml_diff>
--- a/Vanguard US/Vanguard-US-KostenBepaling.xlsx
+++ b/Vanguard US/Vanguard-US-KostenBepaling.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7c741cee80ec8cf3/Financieel/IndexFondsenOnderzoek/KeuzeWelkIndexFonds/OnderzoekPerFonds/Vanguard US/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="901" documentId="13_ncr:1_{1145E7EB-B52A-4035-9DB0-6756A4D32375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{434C35BA-9E86-4B6C-8399-046E74973CA7}"/>
+  <xr:revisionPtr revIDLastSave="924" documentId="13_ncr:1_{1145E7EB-B52A-4035-9DB0-6756A4D32375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D63CF856-476C-428B-8983-F75AE76EC493}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MarketCap" sheetId="7" r:id="rId1"/>
@@ -198,7 +198,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="73">
   <si>
     <t>Dividend income</t>
   </si>
@@ -377,21 +377,6 @@
     <t>VTI-VXUS cheaper</t>
   </si>
   <si>
-    <t>VT leak</t>
-  </si>
-  <si>
-    <t>VTI-VXUS leak</t>
-  </si>
-  <si>
-    <t>Leakage shouldn't be different?</t>
-  </si>
-  <si>
-    <t>VT leak costs</t>
-  </si>
-  <si>
-    <t>VTI-VXUS leak costs</t>
-  </si>
-  <si>
     <t>Index data</t>
   </si>
   <si>
@@ -401,18 +386,6 @@
     <t>CRSP US Total Market Index</t>
   </si>
   <si>
-    <t>2019-2020</t>
-  </si>
-  <si>
-    <t>VXUS</t>
-  </si>
-  <si>
-    <t>Us lager</t>
-  </si>
-  <si>
-    <t>Rest hoger</t>
-  </si>
-  <si>
     <t>Europe</t>
   </si>
   <si>
@@ -422,25 +395,28 @@
     <t>Emerging</t>
   </si>
   <si>
-    <t>VT Lek</t>
-  </si>
-  <si>
-    <t>VTI-VXUS Lek</t>
-  </si>
-  <si>
-    <t>Gemiddeld</t>
-  </si>
-  <si>
-    <t>VXUS Lek</t>
-  </si>
-  <si>
     <t>US</t>
   </si>
   <si>
     <t>Non-US</t>
   </si>
   <si>
-    <t>Verdeling regios</t>
+    <t>VT Leakage</t>
+  </si>
+  <si>
+    <t>Avg</t>
+  </si>
+  <si>
+    <t>VTI-VXUS Leakage</t>
+  </si>
+  <si>
+    <t>Regions</t>
+  </si>
+  <si>
+    <t>VXUS Leakage</t>
+  </si>
+  <si>
+    <t>TODO!</t>
   </si>
 </sst>
 </file>
@@ -895,7 +871,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7D6687D-2650-40D8-BB0F-4784280BA24F}">
   <dimension ref="B2:H31"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -918,7 +894,7 @@
         <v>75163286</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H2" s="3"/>
     </row>
@@ -934,7 +910,7 @@
         <v>0.57709806620216153</v>
       </c>
       <c r="F3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -954,7 +930,7 @@
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C6" s="7">
         <v>44358982</v>
@@ -1029,25 +1005,15 @@
       <c r="F13" s="6"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C14" s="5">
-        <f>VT!J12</f>
-        <v>4.6003640353216309E-2</v>
-      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="6"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C15" s="33">
-        <f>D4*VXUS!J12</f>
-        <v>3.2558816912183416E-2</v>
-      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="33"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="6"/>
@@ -1060,37 +1026,22 @@
       <c r="F16" s="6"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" s="4">
-        <f>VT!J13</f>
-        <v>1.1840408681430441E-3</v>
-      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="4"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="4">
-        <f>D4*VXUS!J13</f>
-        <v>1.0241594364176197E-3</v>
-      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="4"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="6"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="4">
-        <f>C17-C18</f>
-        <v>1.5988143172542446E-4</v>
-      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="4"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="6"/>
@@ -1103,58 +1054,19 @@
       <c r="F20" s="6"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="32" t="s">
-        <v>61</v>
-      </c>
+      <c r="B22" s="32"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="32"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>67</v>
-      </c>
-    </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>68</v>
-      </c>
-      <c r="C25" s="5">
-        <f>AVERAGE(VXUS!H12:I12)</f>
-        <v>9.1049977708263397E-2</v>
-      </c>
+      <c r="C25" s="5"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26" s="5">
-        <f>AVERAGE(VT!H12:I12)</f>
-        <v>5.2625313795850268E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>69</v>
-      </c>
-      <c r="C28">
-        <v>0.82759285222883883</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>70</v>
-      </c>
-      <c r="C29">
-        <f>1/C28</f>
-        <v>1.2083236307646221</v>
-      </c>
+      <c r="C26" s="5"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="3">
-        <f>C25*D4*C29</f>
-        <v>4.6526757138336844E-2</v>
-      </c>
+      <c r="B31" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1164,15 +1076,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F89DD999-D8B8-49AB-8483-F245C54FCD05}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
     <col min="9" max="9" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1196,12 +1106,12 @@
         <v>2020</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B2" s="5">
         <f>VT!D13</f>
@@ -1235,35 +1145,69 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B3" s="5">
-        <f>B9*B8</f>
+        <f t="shared" ref="B3:G3" si="0">B10*B8</f>
         <v>8.9284937543773356E-4</v>
       </c>
       <c r="C3" s="5">
-        <f>C9*C8</f>
+        <f t="shared" si="0"/>
         <v>1.0259972072065302E-3</v>
       </c>
       <c r="D3" s="5">
-        <f>D9*D8</f>
+        <f t="shared" si="0"/>
         <v>1.1168689211553851E-3</v>
       </c>
       <c r="E3" s="5">
-        <f>E9*E8</f>
+        <f t="shared" si="0"/>
         <v>1.0934732621786607E-3</v>
       </c>
       <c r="F3" s="5">
-        <f>F9*F8</f>
+        <f t="shared" si="0"/>
         <v>1.3907721488072657E-3</v>
       </c>
       <c r="G3" s="5">
-        <f>G9*G8</f>
+        <f t="shared" si="0"/>
         <v>1.1751272214198924E-3</v>
       </c>
       <c r="I3" s="9">
         <f>AVERAGE(B3:G3)</f>
         <v>1.1158480227009113E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="5">
+        <f>B2-B3</f>
+        <v>-1.0429124149611874E-5</v>
+      </c>
+      <c r="C4" s="5">
+        <f t="shared" ref="C4:G4" si="1">C2-C3</f>
+        <v>-1.8588222404747334E-5</v>
+      </c>
+      <c r="D4" s="5">
+        <f t="shared" si="1"/>
+        <v>-4.6558588645464983E-5</v>
+      </c>
+      <c r="E4" s="5">
+        <f t="shared" si="1"/>
+        <v>4.1662971820029628E-4</v>
+      </c>
+      <c r="F4" s="5">
+        <f t="shared" si="1"/>
+        <v>8.7255499118622359E-5</v>
+      </c>
+      <c r="G4" s="5">
+        <f t="shared" si="1"/>
+        <v>-1.915220946629775E-5</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="9">
+        <f t="shared" ref="I4" si="2">I2-I3</f>
+        <v>6.8192845442132874E-5</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1277,7 +1221,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -1288,7 +1232,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="B7" s="33">
         <v>0.52400000000000002</v>
@@ -1311,67 +1255,76 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="B8" s="33">
         <f>100%-B7</f>
         <v>0.47599999999999998</v>
       </c>
       <c r="C8" s="33">
-        <f t="shared" ref="C8:G8" si="0">100%-C7</f>
+        <f t="shared" ref="C8:G8" si="3">100%-C7</f>
         <v>0.47899999999999998</v>
       </c>
       <c r="D8" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.48399999999999999</v>
       </c>
       <c r="E8" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.45399999999999996</v>
       </c>
       <c r="F8" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.45299999999999996</v>
       </c>
       <c r="G8" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.43100000000000005</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B9" s="5">
+      <c r="A9" s="1"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="5">
         <f>VXUS!D13</f>
         <v>1.8757339820120453E-3</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C10" s="5">
         <f>VXUS!E13</f>
         <v>2.141956591245366E-3</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D10" s="5">
         <f>VXUS!F13</f>
         <v>2.3075804156102997E-3</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E10" s="5">
         <f>VXUS!G13</f>
         <v>2.4085314144904422E-3</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F10" s="5">
         <f>VXUS!H13</f>
         <v>3.0701371938350241E-3</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G10" s="5">
         <f>VXUS!I13</f>
         <v>2.7265132747561305E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E10" s="5"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I13" s="4"/>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E11" s="5"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I14" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1784,9 +1737,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A50C80A-B9F0-42B2-B14F-324E5B39F7D5}">
   <dimension ref="B2:L41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2308,9 +2259,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEF67C86-3C15-44BC-82E9-B79CA13DEE16}">
   <dimension ref="B2:L34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2831,9 +2780,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BFC4B1D-6D6E-4BBB-9C04-D64B6974E845}">
-  <dimension ref="B2:I26"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2843,9 +2794,14 @@
     <col min="7" max="7" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C2" s="1">
         <v>2019</v>
@@ -2860,7 +2816,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>15</v>
       </c>
@@ -2871,7 +2827,7 @@
       <c r="E3" s="34"/>
       <c r="F3" s="34"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>34</v>
       </c>
@@ -2882,7 +2838,7 @@
       <c r="E4" s="34"/>
       <c r="F4" s="34"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>42</v>
       </c>
@@ -2899,13 +2855,13 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>15</v>
       </c>
@@ -2916,7 +2872,7 @@
       <c r="E9" s="34"/>
       <c r="F9" s="34"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>34</v>
       </c>
@@ -2927,7 +2883,7 @@
       <c r="E10" s="34"/>
       <c r="F10" s="34"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>42</v>
       </c>
@@ -2944,13 +2900,13 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>15</v>
       </c>
@@ -2961,7 +2917,7 @@
       <c r="E15" s="34"/>
       <c r="F15" s="34"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>34</v>
       </c>

</xml_diff>